<commit_message>
AVS lab5 graphics added
</commit_message>
<xml_diff>
--- a/AVS/lab5/OpenMP.xlsx
+++ b/AVS/lab5/OpenMP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\GithubProjects\SibSUTIS5semester\AVS\lab5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DE31FC1-D5AE-4815-9313-2CB2E8179C03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19B8120C-19EA-4122-8897-62D13543DADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -634,7 +634,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Speedup</a:t>
+              <a:t>OpenMP</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -677,6 +677,17 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>OpenMP!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>500x500</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -2048,7 +2059,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P30" sqref="P30"/>
+      <selection activeCell="W12" sqref="W12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>